<commit_message>
Forced Retrofit updated: reduced peak Ncap, relaxed 2GW/yr constraint
</commit_message>
<xml_diff>
--- a/suppxls/Scen_ELC_EAF_REFIT_Forced.xlsx
+++ b/suppxls/Scen_ELC_EAF_REFIT_Forced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9102B99B-C76E-40BF-92B3-6B87A506CAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7C5D08-A4CD-482B-9BAE-533C1B2AAB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="-16950" windowWidth="24630" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define REFIT" sheetId="2" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="44">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -185,6 +185,36 @@
   <si>
     <t>NCAP_TLIFE</t>
   </si>
+  <si>
+    <t>~UC_Sets: R_E: REGION1</t>
+  </si>
+  <si>
+    <t>~UC_Sets: T_E:</t>
+  </si>
+  <si>
+    <t>~UC_T</t>
+  </si>
+  <si>
+    <t>UC_N</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>UC_NCAP</t>
+  </si>
+  <si>
+    <t>UC_RHSRT</t>
+  </si>
+  <si>
+    <t>UCNCAP_REAF</t>
+  </si>
+  <si>
+    <t>*-REAF</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
 </sst>
 </file>
 
@@ -194,7 +224,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,8 +362,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +419,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,7 +565,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -513,6 +574,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="97" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="97"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="97" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="97" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="97" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="97" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="97" applyFont="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="20% - Accent5 2" xfId="44" xr:uid="{2E09701F-C8AC-44F3-9A2D-DF9315D4D18B}"/>
@@ -777,25 +848,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3359999995723331</c:v>
+                  <c:v>3.565999999367333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.565999999367333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2709999998440002</c:v>
+                  <c:v>2.9910000000573334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.071999999320667</c:v>
+                  <c:v>2.6200000005480004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5610000012556666</c:v>
+                  <c:v>3.1719999998260002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4000005295383744E-10</c:v>
+                  <c:v>1.8910000001939999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.4000005295383744E-10</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1997,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:BG79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" topLeftCell="F29" workbookViewId="0">
+      <selection activeCell="X55" sqref="X55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4967,7 +5038,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
         <v>3</v>
       </c>
@@ -4991,19 +5062,19 @@
       </c>
       <c r="I33" s="3">
         <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="28"/>
         <v>1.2799999997866667</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <f t="shared" si="28"/>
         <v>1.2799999997866667</v>
       </c>
-      <c r="K33" s="3">
+      <c r="L33" s="3">
         <f t="shared" si="28"/>
         <v>1.2799999997866667</v>
-      </c>
-      <c r="L33" s="3">
-        <f t="shared" si="28"/>
-        <v>0</v>
       </c>
       <c r="M33" s="3">
         <f t="shared" si="28"/>
@@ -5020,10 +5091,10 @@
         <v>2045</v>
       </c>
       <c r="R33">
-        <v>2027</v>
+        <v>2028</v>
       </c>
     </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>10</v>
       </c>
@@ -5079,7 +5150,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>11</v>
       </c>
@@ -5135,7 +5206,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C36" s="5" t="s">
         <v>12</v>
       </c>
@@ -5163,15 +5234,15 @@
       </c>
       <c r="J36" s="3">
         <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" si="28"/>
         <v>1.2219999995926667</v>
       </c>
-      <c r="K36" s="3">
+      <c r="L36" s="3">
         <f t="shared" si="28"/>
         <v>0.61100000040733327</v>
-      </c>
-      <c r="L36" s="3">
-        <f t="shared" si="28"/>
-        <v>0</v>
       </c>
       <c r="M36" s="3">
         <f t="shared" si="28"/>
@@ -5188,10 +5259,10 @@
         <v>2050</v>
       </c>
       <c r="R36">
-        <v>2028</v>
+        <v>2029</v>
       </c>
     </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
@@ -5247,7 +5318,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C38" s="5" t="s">
         <v>14</v>
       </c>
@@ -5263,7 +5334,7 @@
       </c>
       <c r="G38" s="3">
         <f t="shared" ref="G38:M38" si="30">IF(G56&lt;0.01,0,G56)</f>
-        <v>0</v>
+        <v>1.229999999795</v>
       </c>
       <c r="H38" s="3">
         <f t="shared" si="30"/>
@@ -5275,7 +5346,7 @@
       </c>
       <c r="J38" s="3">
         <f t="shared" si="30"/>
-        <v>1.229999999795</v>
+        <v>0</v>
       </c>
       <c r="K38" s="3">
         <f t="shared" si="30"/>
@@ -5300,10 +5371,10 @@
         <v>2045</v>
       </c>
       <c r="R38">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>15</v>
       </c>
@@ -5359,7 +5430,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>16</v>
       </c>
@@ -5415,14 +5486,14 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -5431,7 +5502,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -5463,7 +5534,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>26</v>
       </c>
@@ -5473,7 +5544,7 @@
       </c>
       <c r="G44" s="3">
         <f t="shared" ref="G44:N44" si="31">SUM(G45:G58)</f>
-        <v>2.3359999995723331</v>
+        <v>3.565999999367333</v>
       </c>
       <c r="H44" s="3">
         <f t="shared" si="31"/>
@@ -5481,30 +5552,30 @@
       </c>
       <c r="I44" s="3">
         <f t="shared" si="31"/>
-        <v>4.2709999998440002</v>
+        <v>2.9910000000573334</v>
       </c>
       <c r="J44" s="3">
         <f t="shared" si="31"/>
-        <v>5.071999999320667</v>
+        <v>2.6200000005480004</v>
       </c>
       <c r="K44" s="3">
         <f t="shared" si="31"/>
-        <v>2.5610000012556666</v>
+        <v>3.1719999998260002</v>
       </c>
       <c r="L44" s="3">
         <f t="shared" si="31"/>
-        <v>6.4000005295383744E-10</v>
+        <v>1.8910000001939999</v>
       </c>
       <c r="M44" s="3">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>6.4000005295383744E-10</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C45" t="str">
         <f t="shared" ref="C45:C58" si="32">C27</f>
         <v>ETCLECAMD-E-REAF</v>
@@ -5548,8 +5619,11 @@
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
+      <c r="S45" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C46" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEGROO-E-REAF</v>
@@ -5593,8 +5667,11 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
+      <c r="S46" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C47" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEKOMA-E-REAF</v>
@@ -5639,7 +5716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C48" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEARNO-E-REAF</v>
@@ -5684,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C49" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEDUVH-E-REAF</v>
@@ -5729,7 +5806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C50" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEHEND-E-REAF</v>
@@ -5774,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C51" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEKEND-E-REAF</v>
@@ -5796,30 +5873,37 @@
       </c>
       <c r="I51" s="3">
         <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="3">
+        <f t="shared" si="35"/>
         <v>1.2799999997866667</v>
       </c>
-      <c r="J51" s="3">
+      <c r="K51" s="3">
         <f t="shared" si="35"/>
         <v>1.2799999997866667</v>
       </c>
-      <c r="K51" s="3">
+      <c r="L51" s="3">
         <f t="shared" si="35"/>
         <v>1.2799999997866667</v>
       </c>
-      <c r="L51" s="3">
+      <c r="M51" s="3">
         <f t="shared" si="35"/>
         <v>6.4000005295383744E-10</v>
       </c>
-      <c r="M51" s="3">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
       <c r="N51" s="3">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
+      <c r="S51" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
     </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C52" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEKRIE-E-REAF</v>
@@ -5863,8 +5947,26 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
+      <c r="S52" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T52" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="U52" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="V52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W52" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="X52" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="53" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C53" t="str">
         <f t="shared" si="32"/>
         <v>ETCLELETH-E-REAF</v>
@@ -5908,8 +6010,26 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
+      <c r="S53" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="U53" s="8">
+        <v>0</v>
+      </c>
+      <c r="V53" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="W53" s="8">
+        <v>3</v>
+      </c>
+      <c r="X53" s="8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="54" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C54" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEMAJD-E-REAF</v>
@@ -5935,16 +6055,16 @@
       </c>
       <c r="J54" s="3">
         <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <f t="shared" si="35"/>
         <v>1.2219999995926667</v>
       </c>
-      <c r="K54" s="3">
+      <c r="L54" s="3">
         <f t="shared" si="35"/>
         <v>0.61100000040733327</v>
       </c>
-      <c r="L54" s="3">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
       <c r="M54" s="3">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -5953,8 +6073,26 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
+      <c r="S54" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="T54" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="U54" s="8">
+        <v>2017</v>
+      </c>
+      <c r="V54" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="W54" s="8">
+        <v>1</v>
+      </c>
+      <c r="X54" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="55" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C55" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEMAJW-E-REAF</v>
@@ -5999,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C56" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEMATI-E-REAF</v>
@@ -6013,7 +6151,7 @@
       </c>
       <c r="G56" s="3">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1.229999999795</v>
       </c>
       <c r="H56" s="3">
         <f t="shared" si="35"/>
@@ -6025,11 +6163,11 @@
       </c>
       <c r="J56" s="3">
         <f t="shared" si="35"/>
-        <v>1.229999999795</v>
+        <v>6.1500005088532816E-10</v>
       </c>
       <c r="K56" s="3">
         <f t="shared" si="35"/>
-        <v>6.1500005088532816E-10</v>
+        <v>0</v>
       </c>
       <c r="L56" s="3">
         <f t="shared" si="35"/>
@@ -6044,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C57" t="str">
         <f t="shared" si="32"/>
         <v>ETCLEMATL-E-REAF</v>
@@ -6089,7 +6227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C58" t="str">
         <f t="shared" si="32"/>
         <v>ETCLETUTU-E-REAF</v>
@@ -6134,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" ref="C60:C73" si="36">C27</f>
         <v>ETCLECAMD-E-REAF</v>
@@ -6179,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C61" t="str">
         <f t="shared" si="36"/>
         <v>ETCLEGROO-E-REAF</v>
@@ -6224,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C62" t="str">
         <f t="shared" si="36"/>
         <v>ETCLEKOMA-E-REAF</v>
@@ -6269,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
         <f t="shared" si="36"/>
         <v>ETCLEARNO-E-REAF</v>
@@ -6314,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C64" t="str">
         <f t="shared" si="36"/>
         <v>ETCLEDUVH-E-REAF</v>
@@ -6426,19 +6564,19 @@
       </c>
       <c r="I66">
         <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="37"/>
         <v>1.2799999997866667</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <f t="shared" si="37"/>
         <v>2.5599999995733334</v>
       </c>
-      <c r="K66">
+      <c r="L66">
         <f t="shared" si="37"/>
         <v>3.8399999993599998</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="37"/>
-        <v>3.84</v>
       </c>
       <c r="M66">
         <f t="shared" si="37"/>
@@ -6565,11 +6703,11 @@
       </c>
       <c r="J69">
         <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="37"/>
         <v>1.2219999995926667</v>
-      </c>
-      <c r="K69">
-        <f t="shared" si="37"/>
-        <v>1.833</v>
       </c>
       <c r="L69">
         <f t="shared" si="37"/>
@@ -6643,19 +6781,19 @@
       </c>
       <c r="G71">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1.229999999795</v>
       </c>
       <c r="H71">
         <f t="shared" si="37"/>
-        <v>1.229999999795</v>
+        <v>2.4599999995899999</v>
       </c>
       <c r="I71">
         <f t="shared" si="37"/>
-        <v>2.4599999995899999</v>
+        <v>3.6899999993849999</v>
       </c>
       <c r="J71">
         <f t="shared" si="37"/>
-        <v>3.6899999993849999</v>
+        <v>3.69</v>
       </c>
       <c r="K71">
         <f t="shared" si="37"/>

</xml_diff>